<commit_message>
Update R004 Acceptance Testing to Traceability Report for MS5
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
+++ b/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\MS5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\toGit\SFT221_GROUP_PROJECT\Documents\Testing\TestsDocuments\ms5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF50FE7-F09A-4854-A0BD-C74A9432BF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664C5556-C3CA-4D59-B56C-42635BBB4C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="150">
   <si>
     <t>Business Requirements</t>
   </si>
@@ -938,18 +938,65 @@
   </si>
   <si>
     <t>Will not be tested in this MS</t>
+  </si>
+  <si>
+    <t>Valid message shown</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CAPACITY REACHED! Go to next closet Route
+Ship on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BLUE LINE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>divert: 8Y, 8Y</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1169,9 +1216,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1185,116 +1232,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1574,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1606,8 +1656,8 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:14" s="31" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:14" s="25" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="11"/>
@@ -1615,22 +1665,22 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="37" t="s">
+      <c r="H2" s="41"/>
+      <c r="I2" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="37" t="s">
+      <c r="J2" s="41"/>
+      <c r="K2" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="39"/>
-      <c r="M2" s="37" t="s">
+      <c r="L2" s="41"/>
+      <c r="M2" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="39"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" spans="1:14" ht="29.4" thickBot="1">
       <c r="A3" s="5" t="s">
@@ -1678,10 +1728,10 @@
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="36" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3">
@@ -1702,10 +1752,16 @@
       <c r="J4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="40" t="s">
+      <c r="K4" s="33" t="s">
         <v>147</v>
       </c>
       <c r="L4" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1713,8 +1769,8 @@
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="3">
         <v>1000</v>
       </c>
@@ -1733,8 +1789,12 @@
       <c r="J5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="41"/>
+      <c r="K5" s="34"/>
       <c r="L5" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="34"/>
+      <c r="N5" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1742,8 +1802,8 @@
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="3">
         <v>-0.1</v>
       </c>
@@ -1762,8 +1822,12 @@
       <c r="J6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="41"/>
+      <c r="K6" s="34"/>
       <c r="L6" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="34"/>
+      <c r="N6" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1771,8 +1835,8 @@
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="3">
         <v>1000.1</v>
       </c>
@@ -1791,20 +1855,24 @@
       <c r="J7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="41"/>
+      <c r="K7" s="34"/>
       <c r="L7" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="23" customFormat="1"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="39" customFormat="1"/>
     <row r="9" spans="1:14" ht="43.2" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="36" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="3">
@@ -1825,10 +1893,16 @@
       <c r="J9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="34" t="s">
         <v>147</v>
       </c>
       <c r="L9" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="N9" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1836,8 +1910,8 @@
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="3">
         <v>0.5</v>
       </c>
@@ -1856,8 +1930,12 @@
       <c r="J10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="41"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M10" s="34"/>
+      <c r="N10" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1865,8 +1943,8 @@
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="3">
         <v>1</v>
       </c>
@@ -1885,8 +1963,12 @@
       <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="41"/>
+      <c r="K11" s="34"/>
       <c r="L11" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M11" s="34"/>
+      <c r="N11" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1894,8 +1976,8 @@
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="25"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="3">
         <v>0.24</v>
       </c>
@@ -1914,8 +1996,12 @@
       <c r="J12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="41"/>
+      <c r="K12" s="34"/>
       <c r="L12" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="34"/>
+      <c r="N12" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1923,8 +2009,8 @@
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="3">
         <v>-0.5</v>
       </c>
@@ -1943,8 +2029,12 @@
       <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="41"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M13" s="34"/>
+      <c r="N13" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1952,8 +2042,8 @@
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -1972,20 +2062,24 @@
       <c r="J14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="41"/>
+      <c r="K14" s="34"/>
       <c r="L14" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" s="23" customFormat="1"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="39" customFormat="1"/>
     <row r="16" spans="1:14">
       <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2006,19 +2100,25 @@
       <c r="J16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="31" t="s">
         <v>139</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="2:12">
+      <c r="M16" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
@@ -2037,17 +2137,21 @@
       <c r="J17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="26"/>
+      <c r="K17" s="32"/>
       <c r="L17" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="2:12">
+      <c r="M17" s="32"/>
+      <c r="N17" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
       <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="3" t="s">
         <v>32</v>
       </c>
@@ -2066,17 +2170,21 @@
       <c r="J18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="26"/>
+      <c r="K18" s="32"/>
       <c r="L18" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="2:12">
+      <c r="M18" s="32"/>
+      <c r="N18" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="3" t="s">
         <v>34</v>
       </c>
@@ -2095,17 +2203,21 @@
       <c r="J19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="26"/>
+      <c r="K19" s="32"/>
       <c r="L19" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="2:12">
+      <c r="M19" s="32"/>
+      <c r="N19" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
       <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2124,17 +2236,21 @@
       <c r="J20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="26"/>
+      <c r="K20" s="32"/>
       <c r="L20" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="2:12">
+      <c r="M20" s="32"/>
+      <c r="N20" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
       <c r="B21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="3" t="s">
         <v>38</v>
       </c>
@@ -2153,17 +2269,21 @@
       <c r="J21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="26"/>
+      <c r="K21" s="32"/>
       <c r="L21" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="2:12">
+      <c r="M21" s="32"/>
+      <c r="N21" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
@@ -2182,17 +2302,21 @@
       <c r="J22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="26"/>
+      <c r="K22" s="32"/>
       <c r="L22" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="2:12">
+      <c r="M22" s="32"/>
+      <c r="N22" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="3" t="s">
         <v>42</v>
       </c>
@@ -2211,17 +2335,21 @@
       <c r="J23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="26"/>
+      <c r="K23" s="32"/>
       <c r="L23" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="2:12">
+      <c r="M23" s="32"/>
+      <c r="N23" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="3" t="s">
         <v>44</v>
       </c>
@@ -2240,17 +2368,21 @@
       <c r="J24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="26"/>
+      <c r="K24" s="32"/>
       <c r="L24" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="2:12">
+      <c r="M24" s="32"/>
+      <c r="N24" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="3" t="s">
         <v>47</v>
       </c>
@@ -2269,20 +2401,24 @@
       <c r="J25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="26"/>
+      <c r="K25" s="32"/>
       <c r="L25" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" s="23" customFormat="1"/>
-    <row r="27" spans="2:12" ht="28.8" customHeight="1">
+      <c r="M25" s="32"/>
+      <c r="N25" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" s="39" customFormat="1"/>
+    <row r="27" spans="2:14" ht="28.8" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="36" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -2306,20 +2442,26 @@
       <c r="K27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L27" s="33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12">
+      <c r="L27" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
       <c r="B28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="25"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="36"/>
       <c r="E28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="24" t="s">
         <v>52</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -2337,16 +2479,22 @@
       <c r="K28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L28" s="33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12">
+      <c r="L28" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
       <c r="B29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="25"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="36"/>
       <c r="E29" s="3" t="s">
         <v>61</v>
       </c>
@@ -2371,13 +2519,19 @@
       <c r="L29" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="2:12">
+      <c r="M29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
       <c r="B30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="25"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="36"/>
       <c r="E30" s="3" t="s">
         <v>64</v>
       </c>
@@ -2402,13 +2556,19 @@
       <c r="L30" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="2:12">
+      <c r="M30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
       <c r="B31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="25"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="36"/>
       <c r="E31" s="3" t="s">
         <v>68</v>
       </c>
@@ -2427,19 +2587,25 @@
       <c r="J31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K31" s="34" t="s">
+      <c r="K31" s="28" t="s">
         <v>137</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="2:12">
+      <c r="M31" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
       <c r="B32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="25"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="14" t="s">
         <v>71</v>
       </c>
@@ -2464,13 +2630,19 @@
       <c r="L32" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="2:12">
+      <c r="M32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
       <c r="B33" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="25"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="36"/>
       <c r="E33" s="3" t="s">
         <v>74</v>
       </c>
@@ -2495,13 +2667,19 @@
       <c r="L33" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="2:12">
+      <c r="M33" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N33" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
       <c r="B34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="25"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="36"/>
       <c r="E34" s="3" t="s">
         <v>56</v>
       </c>
@@ -2526,13 +2704,19 @@
       <c r="L34" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="2:12">
+      <c r="M34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N34" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
       <c r="B35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="25"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="3" t="s">
         <v>80</v>
       </c>
@@ -2551,19 +2735,25 @@
       <c r="J35" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K35" s="35" t="s">
+      <c r="K35" s="29" t="s">
         <v>138</v>
       </c>
       <c r="L35" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="2:12">
+      <c r="M35" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
       <c r="B36" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="25"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="15" t="s">
         <v>82</v>
       </c>
@@ -2582,22 +2772,28 @@
       <c r="J36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K36" s="35" t="s">
+      <c r="K36" s="29" t="s">
         <v>138</v>
       </c>
       <c r="L36" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" s="23" customFormat="1"/>
-    <row r="38" spans="2:12" ht="43.2">
+      <c r="M36" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N36" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" s="39" customFormat="1"/>
+    <row r="38" spans="2:14" ht="43.2">
       <c r="B38" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="24" t="s">
         <v>85</v>
       </c>
       <c r="E38" s="16" t="s">
@@ -2624,13 +2820,19 @@
       <c r="L38" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" s="23" customFormat="1"/>
-    <row r="40" spans="2:12" ht="15" customHeight="1">
+      <c r="M38" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="N38" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" s="39" customFormat="1"/>
+    <row r="40" spans="2:14" ht="15" customHeight="1">
       <c r="B40" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="23" t="s">
         <v>89</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2660,16 +2862,22 @@
       <c r="L40" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" s="23" customFormat="1"/>
-    <row r="42" spans="2:12" ht="14.4" customHeight="1">
+      <c r="M40" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" s="39" customFormat="1"/>
+    <row r="42" spans="2:14" ht="14.4" customHeight="1">
       <c r="B42" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="36" t="s">
         <v>95</v>
       </c>
       <c r="E42" s="3">
@@ -2690,19 +2898,25 @@
       <c r="J42" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K42" s="41" t="s">
+      <c r="K42" s="34" t="s">
         <v>147</v>
       </c>
       <c r="L42" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="2:12">
+      <c r="M42" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14">
       <c r="B43" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
       <c r="E43" s="3">
         <v>1</v>
       </c>
@@ -2721,17 +2935,21 @@
       <c r="J43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="41"/>
+      <c r="K43" s="34"/>
       <c r="L43" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="44" spans="2:12">
+      <c r="M43" s="34"/>
+      <c r="N43" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
       <c r="B44" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
       <c r="E44" s="3">
         <v>1000</v>
       </c>
@@ -2750,17 +2968,21 @@
       <c r="J44" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K44" s="41"/>
+      <c r="K44" s="34"/>
       <c r="L44" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="45" spans="2:12">
+      <c r="M44" s="34"/>
+      <c r="N44" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
       <c r="B45" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
       <c r="E45" s="3">
         <v>1234.3209999999999</v>
       </c>
@@ -2779,17 +3001,21 @@
       <c r="J45" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K45" s="41"/>
+      <c r="K45" s="34"/>
       <c r="L45" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="2:12">
+      <c r="M45" s="34"/>
+      <c r="N45" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14">
       <c r="B46" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
       <c r="E46" s="19" t="s">
         <v>101</v>
       </c>
@@ -2808,12 +3034,16 @@
       <c r="J46" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K46" s="41"/>
+      <c r="K46" s="34"/>
       <c r="L46" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" s="2" customFormat="1">
+      <c r="M46" s="34"/>
+      <c r="N46" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" s="2" customFormat="1">
       <c r="B47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2822,14 +3052,14 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="2:12" ht="14.4" customHeight="1">
+    <row r="48" spans="2:14" ht="14.4" customHeight="1">
       <c r="B48" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="36" t="s">
         <v>18</v>
       </c>
       <c r="E48" s="3">
@@ -2850,19 +3080,25 @@
       <c r="J48" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K48" s="41" t="s">
+      <c r="K48" s="34" t="s">
         <v>147</v>
       </c>
       <c r="L48" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="2:12">
+      <c r="M48" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="N48" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14">
       <c r="B49" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="26"/>
-      <c r="D49" s="25"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="36"/>
       <c r="E49" s="3">
         <v>0.5</v>
       </c>
@@ -2881,17 +3117,21 @@
       <c r="J49" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K49" s="24"/>
+      <c r="K49" s="35"/>
       <c r="L49" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="2:12">
+      <c r="M49" s="35"/>
+      <c r="N49" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14">
       <c r="B50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="25"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="36"/>
       <c r="E50" s="3">
         <v>1</v>
       </c>
@@ -2910,17 +3150,21 @@
       <c r="J50" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K50" s="24"/>
+      <c r="K50" s="35"/>
       <c r="L50" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="51" spans="2:12">
+      <c r="M50" s="35"/>
+      <c r="N50" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14">
       <c r="B51" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="25"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="36"/>
       <c r="E51" s="3">
         <v>0.75</v>
       </c>
@@ -2939,17 +3183,21 @@
       <c r="J51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K51" s="24"/>
+      <c r="K51" s="35"/>
       <c r="L51" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="52" spans="2:12">
+      <c r="M51" s="35"/>
+      <c r="N51" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14">
       <c r="B52" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="25"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="36"/>
       <c r="E52" s="19" t="s">
         <v>108</v>
       </c>
@@ -2968,20 +3216,24 @@
       <c r="J52" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K52" s="24"/>
+      <c r="K52" s="35"/>
       <c r="L52" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" s="23" customFormat="1"/>
-    <row r="54" spans="2:12" ht="14.4" customHeight="1">
+      <c r="M52" s="35"/>
+      <c r="N52" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" s="39" customFormat="1"/>
+    <row r="54" spans="2:14" ht="14.4" customHeight="1">
       <c r="B54" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D54" s="36" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="19" t="s">
@@ -3002,19 +3254,25 @@
       <c r="J54" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K54" s="36" t="s">
+      <c r="K54" s="31" t="s">
         <v>139</v>
       </c>
       <c r="L54" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="55" spans="2:12">
+      <c r="M54" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="N54" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14">
       <c r="B55" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
       <c r="E55" s="19" t="s">
         <v>113</v>
       </c>
@@ -3033,17 +3291,21 @@
       <c r="J55" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="36"/>
+      <c r="K55" s="31"/>
       <c r="L55" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="56" spans="2:12">
+      <c r="M55" s="31"/>
+      <c r="N55" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14">
       <c r="B56" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
       <c r="E56" s="19" t="s">
         <v>115</v>
       </c>
@@ -3062,17 +3324,21 @@
       <c r="J56" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K56" s="36"/>
+      <c r="K56" s="31"/>
       <c r="L56" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="57" spans="2:12">
+      <c r="M56" s="31"/>
+      <c r="N56" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14">
       <c r="B57" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
       <c r="E57" s="19" t="s">
         <v>117</v>
       </c>
@@ -3091,17 +3357,21 @@
       <c r="J57" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="K57" s="36"/>
+      <c r="K57" s="31"/>
       <c r="L57" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="58" spans="2:12">
+      <c r="M57" s="31"/>
+      <c r="N57" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14">
       <c r="B58" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
       <c r="E58" s="19" t="s">
         <v>120</v>
       </c>
@@ -3120,17 +3390,21 @@
       <c r="J58" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K58" s="36"/>
+      <c r="K58" s="31"/>
       <c r="L58" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="59" spans="2:12">
+      <c r="M58" s="31"/>
+      <c r="N58" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14">
       <c r="B59" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
       <c r="E59" s="19" t="s">
         <v>122</v>
       </c>
@@ -3149,24 +3423,28 @@
       <c r="J59" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K59" s="36"/>
+      <c r="K59" s="31"/>
       <c r="L59" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="60" spans="2:12" s="32" customFormat="1"/>
-    <row r="61" spans="2:12" s="31" customFormat="1" ht="14.4" customHeight="1">
+      <c r="M59" s="31"/>
+      <c r="N59" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" s="26" customFormat="1"/>
+    <row r="61" spans="2:14" s="25" customFormat="1" ht="14.4" customHeight="1">
       <c r="B61" s="11"/>
-      <c r="C61" s="27" t="s">
+      <c r="C61" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="27" t="s">
+      <c r="D61" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E61" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F61" s="30" t="s">
+      <c r="F61" s="23" t="s">
         <v>58</v>
       </c>
       <c r="G61" s="19" t="s">
@@ -3182,14 +3460,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="2:12" s="31" customFormat="1">
+    <row r="62" spans="2:14" s="25" customFormat="1">
       <c r="B62" s="11"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="30" t="s">
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="F62" s="30" t="s">
+      <c r="F62" s="23" t="s">
         <v>66</v>
       </c>
       <c r="G62" s="19" t="s">
@@ -3205,14 +3483,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="2:12" s="31" customFormat="1">
+    <row r="63" spans="2:14" s="25" customFormat="1">
       <c r="B63" s="11"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="30" t="s">
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F63" s="30" t="s">
+      <c r="F63" s="23" t="s">
         <v>54</v>
       </c>
       <c r="G63" s="19" t="s">
@@ -3228,14 +3506,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="2:12" s="31" customFormat="1">
+    <row r="64" spans="2:14" s="25" customFormat="1">
       <c r="B64" s="11"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="30" t="s">
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="F64" s="30" t="s">
+      <c r="F64" s="23" t="s">
         <v>134</v>
       </c>
       <c r="G64" s="19" t="s">
@@ -3251,14 +3529,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="2:12" s="31" customFormat="1" ht="28.05" customHeight="1">
+    <row r="65" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B65" s="11"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="30" t="s">
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="F65" s="30" t="s">
+      <c r="F65" s="23" t="s">
         <v>135</v>
       </c>
       <c r="G65" s="19" t="s">
@@ -3274,14 +3552,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="2:12" s="31" customFormat="1" ht="28.05" customHeight="1">
+    <row r="66" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B66" s="11"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="30" t="s">
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="F66" s="30" t="s">
+      <c r="F66" s="23" t="s">
         <v>135</v>
       </c>
       <c r="G66" s="19" t="s">
@@ -3297,14 +3575,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="2:12" s="31" customFormat="1" ht="43.2">
+    <row r="67" spans="2:14" s="25" customFormat="1" ht="43.2">
       <c r="B67" s="11"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="30" t="s">
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="F67" s="30" t="s">
+      <c r="F67" s="23" t="s">
         <v>136</v>
       </c>
       <c r="G67" s="19" t="s">
@@ -3320,14 +3598,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="2:12" s="31" customFormat="1">
+    <row r="68" spans="2:14" s="25" customFormat="1">
       <c r="B68" s="11"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="30" t="s">
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F68" s="30" t="s">
+      <c r="F68" s="23" t="s">
         <v>91</v>
       </c>
       <c r="G68" s="19" t="s">
@@ -3343,18 +3621,18 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="2:12" s="28" customFormat="1"/>
-    <row r="70" spans="2:12" ht="14.4" customHeight="1">
-      <c r="C70" s="27" t="s">
+    <row r="69" spans="2:14" s="38" customFormat="1"/>
+    <row r="70" spans="2:14" ht="14.4" customHeight="1">
+      <c r="C70" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="D70" s="27" t="s">
+      <c r="D70" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="E70" s="30" t="s">
+      <c r="E70" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="30" t="s">
+      <c r="F70" s="23" t="s">
         <v>58</v>
       </c>
       <c r="G70" s="19" t="s">
@@ -3375,14 +3653,20 @@
       <c r="L70" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="71" spans="2:12">
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="30" t="s">
+      <c r="M70" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="N70" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14">
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="F71" s="30" t="s">
+      <c r="F71" s="23" t="s">
         <v>66</v>
       </c>
       <c r="G71" s="19" t="s">
@@ -3397,20 +3681,26 @@
       <c r="J71" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="K71" s="30" t="s">
+      <c r="K71" s="23" t="s">
         <v>66</v>
       </c>
       <c r="L71" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="2:12">
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="30" t="s">
+      <c r="M71" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="N71" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14">
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F72" s="30" t="s">
+      <c r="F72" s="23" t="s">
         <v>54</v>
       </c>
       <c r="G72" s="19" t="s">
@@ -3425,20 +3715,26 @@
       <c r="J72" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="K72" s="30" t="s">
+      <c r="K72" s="23" t="s">
         <v>54</v>
       </c>
       <c r="L72" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="2:12" ht="57.6">
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="30" t="s">
+      <c r="M72" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="N72" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14" ht="57.6">
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="F73" s="30" t="s">
+      <c r="F73" s="23" t="s">
         <v>134</v>
       </c>
       <c r="G73" s="19" t="s">
@@ -3453,20 +3749,26 @@
       <c r="J73" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="K73" s="30" t="s">
+      <c r="K73" s="23" t="s">
         <v>144</v>
       </c>
       <c r="L73" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="74" spans="2:12" ht="28.8">
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="30" t="s">
+      <c r="M73" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N73" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" ht="28.8">
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="F74" s="30" t="s">
+      <c r="F74" s="23" t="s">
         <v>135</v>
       </c>
       <c r="G74" s="19" t="s">
@@ -3481,20 +3783,26 @@
       <c r="J74" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="K74" s="30" t="s">
+      <c r="K74" s="23" t="s">
         <v>145</v>
       </c>
       <c r="L74" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="75" spans="2:12" ht="28.8">
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="30" t="s">
+      <c r="M74" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="N74" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" ht="28.8">
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="F75" s="30" t="s">
+      <c r="F75" s="23" t="s">
         <v>135</v>
       </c>
       <c r="G75" s="19" t="s">
@@ -3509,20 +3817,26 @@
       <c r="J75" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="K75" s="30" t="s">
+      <c r="K75" s="23" t="s">
         <v>146</v>
       </c>
       <c r="L75" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="76" spans="2:12" ht="43.2">
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="30" t="s">
+      <c r="M75" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="N75" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14" ht="43.2">
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="F76" s="30" t="s">
+      <c r="F76" s="23" t="s">
         <v>136</v>
       </c>
       <c r="G76" s="19" t="s">
@@ -3537,20 +3851,26 @@
       <c r="J76" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="K76" s="30" t="s">
+      <c r="K76" s="23" t="s">
         <v>145</v>
       </c>
       <c r="L76" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="77" spans="2:12">
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="30" t="s">
+      <c r="M76" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="N76" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14">
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F77" s="30" t="s">
+      <c r="F77" s="23" t="s">
         <v>91</v>
       </c>
       <c r="G77" s="19" t="s">
@@ -3571,34 +3891,31 @@
       <c r="L77" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="2:12">
+      <c r="M77" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="N77" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14">
       <c r="C78" s="4"/>
-      <c r="D78" s="31"/>
-    </row>
-    <row r="79" spans="2:12">
+      <c r="D78" s="25"/>
+    </row>
+    <row r="79" spans="2:14">
       <c r="C79" s="4"/>
-      <c r="D79" s="31"/>
+      <c r="D79" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="K16:K25"/>
-    <mergeCell ref="K54:K59"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K9:K14"/>
-    <mergeCell ref="K42:K46"/>
-    <mergeCell ref="K48:K52"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="C61:C68"/>
-    <mergeCell ref="D61:D68"/>
-    <mergeCell ref="C70:C77"/>
-    <mergeCell ref="D70:D77"/>
-    <mergeCell ref="A69:XFD69"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C16:C25"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="C42:C46"/>
+  <mergeCells count="42">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="A15:XFD15"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="M9:M14"/>
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="C54:C59"/>
     <mergeCell ref="D4:D7"/>
@@ -3612,12 +3929,27 @@
     <mergeCell ref="A39:XFD39"/>
     <mergeCell ref="A41:XFD41"/>
     <mergeCell ref="A53:XFD53"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M16:M25"/>
+    <mergeCell ref="M42:M46"/>
+    <mergeCell ref="M48:M52"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C16:C25"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="C61:C68"/>
+    <mergeCell ref="D61:D68"/>
+    <mergeCell ref="C70:C77"/>
+    <mergeCell ref="D70:D77"/>
+    <mergeCell ref="A69:XFD69"/>
+    <mergeCell ref="M54:M59"/>
+    <mergeCell ref="K16:K25"/>
+    <mergeCell ref="K54:K59"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K9:K14"/>
+    <mergeCell ref="K42:K46"/>
+    <mergeCell ref="K48:K52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Updated matrix traceability file
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
+++ b/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\toGit\SFT221_GROUP_PROJECT\Documents\Testing\TestsDocuments\ms5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zohrab Zeynalli\OneDrive\Documents\SENECA\2semester\SFT221\SFT221_GROUP_PROJECT\Documents\Testing\TestsDocuments\ms5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664C5556-C3CA-4D59-B56C-42635BBB4C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42122AC-A38C-4B53-B510-66E22604AFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="156">
   <si>
     <t>Business Requirements</t>
   </si>
@@ -978,18 +991,43 @@
       </rPr>
       <t>divert: 8Y, 8Y</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  Invalid size                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">              Invalid weight (must be 1-1000 Kg.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       Invalid destination format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Ship on BLUE LINE, no diversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Ship on GREEN LINE, divert: 8Y, 8Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Thanks for shipping with Seneca!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1216,9 +1254,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1232,116 +1270,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1624,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M73" sqref="M73"/>
+    <sheetView tabSelected="1" topLeftCell="I53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N63" sqref="N63:N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1665,22 +1706,22 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="40" t="s">
+      <c r="H2" s="33"/>
+      <c r="I2" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="40" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="41"/>
-      <c r="M2" s="40" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="41"/>
+      <c r="N2" s="33"/>
     </row>
     <row r="3" spans="1:14" ht="29.4" thickBot="1">
       <c r="A3" s="5" t="s">
@@ -1728,10 +1769,10 @@
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="37" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3">
@@ -1752,13 +1793,13 @@
       <c r="J4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="35" t="s">
         <v>147</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="35" t="s">
         <v>147</v>
       </c>
       <c r="N4" s="19" t="s">
@@ -1769,8 +1810,8 @@
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="3">
         <v>1000</v>
       </c>
@@ -1789,11 +1830,11 @@
       <c r="J5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="34"/>
+      <c r="K5" s="36"/>
       <c r="L5" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="34"/>
+      <c r="M5" s="36"/>
       <c r="N5" s="19" t="s">
         <v>96</v>
       </c>
@@ -1802,8 +1843,8 @@
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="3">
         <v>-0.1</v>
       </c>
@@ -1822,11 +1863,11 @@
       <c r="J6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="34"/>
+      <c r="K6" s="36"/>
       <c r="L6" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M6" s="34"/>
+      <c r="M6" s="36"/>
       <c r="N6" s="19" t="s">
         <v>96</v>
       </c>
@@ -1835,8 +1876,8 @@
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="3">
         <v>1000.1</v>
       </c>
@@ -1855,24 +1896,24 @@
       <c r="J7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="34"/>
+      <c r="K7" s="36"/>
       <c r="L7" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M7" s="34"/>
+      <c r="M7" s="36"/>
       <c r="N7" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="39" customFormat="1"/>
+    <row r="8" spans="1:14" s="34" customFormat="1"/>
     <row r="9" spans="1:14" ht="43.2" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="37" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="3">
@@ -1893,13 +1934,13 @@
       <c r="J9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="K9" s="36" t="s">
         <v>147</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="M9" s="36" t="s">
         <v>147</v>
       </c>
       <c r="N9" s="19" t="s">
@@ -1910,8 +1951,8 @@
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="3">
         <v>0.5</v>
       </c>
@@ -1930,11 +1971,11 @@
       <c r="J10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="34"/>
+      <c r="K10" s="36"/>
       <c r="L10" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="34"/>
+      <c r="M10" s="36"/>
       <c r="N10" s="19" t="s">
         <v>96</v>
       </c>
@@ -1943,8 +1984,8 @@
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="3">
         <v>1</v>
       </c>
@@ -1963,11 +2004,11 @@
       <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="34"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M11" s="34"/>
+      <c r="M11" s="36"/>
       <c r="N11" s="19" t="s">
         <v>96</v>
       </c>
@@ -1976,8 +2017,8 @@
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="3">
         <v>0.24</v>
       </c>
@@ -1996,11 +2037,11 @@
       <c r="J12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="34"/>
+      <c r="K12" s="36"/>
       <c r="L12" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M12" s="34"/>
+      <c r="M12" s="36"/>
       <c r="N12" s="19" t="s">
         <v>96</v>
       </c>
@@ -2009,8 +2050,8 @@
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="3">
         <v>-0.5</v>
       </c>
@@ -2029,11 +2070,11 @@
       <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="36"/>
       <c r="L13" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M13" s="34"/>
+      <c r="M13" s="36"/>
       <c r="N13" s="19" t="s">
         <v>96</v>
       </c>
@@ -2042,8 +2083,8 @@
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="36"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -2062,24 +2103,24 @@
       <c r="J14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="34"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M14" s="34"/>
+      <c r="M14" s="36"/>
       <c r="N14" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="39" customFormat="1"/>
+    <row r="15" spans="1:14" s="34" customFormat="1"/>
     <row r="16" spans="1:14">
       <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="39" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2100,13 +2141,13 @@
       <c r="J16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="31" t="s">
+      <c r="K16" s="41" t="s">
         <v>139</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M16" s="31" t="s">
+      <c r="M16" s="41" t="s">
         <v>139</v>
       </c>
       <c r="N16" s="19" t="s">
@@ -2117,8 +2158,8 @@
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
@@ -2137,11 +2178,11 @@
       <c r="J17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="32"/>
+      <c r="K17" s="38"/>
       <c r="L17" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M17" s="32"/>
+      <c r="M17" s="38"/>
       <c r="N17" s="19" t="s">
         <v>96</v>
       </c>
@@ -2150,8 +2191,8 @@
       <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="3" t="s">
         <v>32</v>
       </c>
@@ -2170,11 +2211,11 @@
       <c r="J18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="32"/>
+      <c r="K18" s="38"/>
       <c r="L18" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M18" s="32"/>
+      <c r="M18" s="38"/>
       <c r="N18" s="19" t="s">
         <v>96</v>
       </c>
@@ -2183,8 +2224,8 @@
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="3" t="s">
         <v>34</v>
       </c>
@@ -2203,11 +2244,11 @@
       <c r="J19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="32"/>
+      <c r="K19" s="38"/>
       <c r="L19" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M19" s="32"/>
+      <c r="M19" s="38"/>
       <c r="N19" s="19" t="s">
         <v>96</v>
       </c>
@@ -2216,8 +2257,8 @@
       <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2236,11 +2277,11 @@
       <c r="J20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="32"/>
+      <c r="K20" s="38"/>
       <c r="L20" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M20" s="32"/>
+      <c r="M20" s="38"/>
       <c r="N20" s="19" t="s">
         <v>96</v>
       </c>
@@ -2249,8 +2290,8 @@
       <c r="B21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="3" t="s">
         <v>38</v>
       </c>
@@ -2269,11 +2310,11 @@
       <c r="J21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="32"/>
+      <c r="K21" s="38"/>
       <c r="L21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M21" s="32"/>
+      <c r="M21" s="38"/>
       <c r="N21" s="19" t="s">
         <v>96</v>
       </c>
@@ -2282,8 +2323,8 @@
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
@@ -2302,11 +2343,11 @@
       <c r="J22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="32"/>
+      <c r="K22" s="38"/>
       <c r="L22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M22" s="32"/>
+      <c r="M22" s="38"/>
       <c r="N22" s="19" t="s">
         <v>96</v>
       </c>
@@ -2315,8 +2356,8 @@
       <c r="B23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="3" t="s">
         <v>42</v>
       </c>
@@ -2335,11 +2376,11 @@
       <c r="J23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="32"/>
+      <c r="K23" s="38"/>
       <c r="L23" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M23" s="32"/>
+      <c r="M23" s="38"/>
       <c r="N23" s="19" t="s">
         <v>96</v>
       </c>
@@ -2348,8 +2389,8 @@
       <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="3" t="s">
         <v>44</v>
       </c>
@@ -2368,11 +2409,11 @@
       <c r="J24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="32"/>
+      <c r="K24" s="38"/>
       <c r="L24" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M24" s="32"/>
+      <c r="M24" s="38"/>
       <c r="N24" s="19" t="s">
         <v>96</v>
       </c>
@@ -2381,8 +2422,8 @@
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="3" t="s">
         <v>47</v>
       </c>
@@ -2401,24 +2442,24 @@
       <c r="J25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="32"/>
+      <c r="K25" s="38"/>
       <c r="L25" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M25" s="32"/>
+      <c r="M25" s="38"/>
       <c r="N25" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="2:14" s="39" customFormat="1"/>
+    <row r="26" spans="2:14" s="34" customFormat="1"/>
     <row r="27" spans="2:14" ht="28.8" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="37" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -2456,8 +2497,8 @@
       <c r="B28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="36"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="3" t="s">
         <v>78</v>
       </c>
@@ -2493,8 +2534,8 @@
       <c r="B29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="36"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="3" t="s">
         <v>61</v>
       </c>
@@ -2530,8 +2571,8 @@
       <c r="B30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="36"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="3" t="s">
         <v>64</v>
       </c>
@@ -2567,8 +2608,8 @@
       <c r="B31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="36"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="3" t="s">
         <v>68</v>
       </c>
@@ -2604,8 +2645,8 @@
       <c r="B32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="36"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="14" t="s">
         <v>71</v>
       </c>
@@ -2641,8 +2682,8 @@
       <c r="B33" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="36"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="3" t="s">
         <v>74</v>
       </c>
@@ -2678,8 +2719,8 @@
       <c r="B34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="36"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="3" t="s">
         <v>56</v>
       </c>
@@ -2715,8 +2756,8 @@
       <c r="B35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="36"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="3" t="s">
         <v>80</v>
       </c>
@@ -2752,8 +2793,8 @@
       <c r="B36" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="36"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="15" t="s">
         <v>82</v>
       </c>
@@ -2785,7 +2826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:14" s="39" customFormat="1"/>
+    <row r="37" spans="2:14" s="34" customFormat="1"/>
     <row r="38" spans="2:14" ht="43.2">
       <c r="B38" s="6" t="s">
         <v>83</v>
@@ -2827,7 +2868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:14" s="39" customFormat="1"/>
+    <row r="39" spans="2:14" s="34" customFormat="1"/>
     <row r="40" spans="2:14" ht="15" customHeight="1">
       <c r="B40" s="6" t="s">
         <v>88</v>
@@ -2869,15 +2910,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:14" s="39" customFormat="1"/>
+    <row r="41" spans="2:14" s="34" customFormat="1"/>
     <row r="42" spans="2:14" ht="14.4" customHeight="1">
       <c r="B42" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D42" s="37" t="s">
         <v>95</v>
       </c>
       <c r="E42" s="3">
@@ -2898,13 +2939,13 @@
       <c r="J42" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K42" s="34" t="s">
+      <c r="K42" s="36" t="s">
         <v>147</v>
       </c>
       <c r="L42" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M42" s="34" t="s">
+      <c r="M42" s="36" t="s">
         <v>147</v>
       </c>
       <c r="N42" s="19" t="s">
@@ -2915,8 +2956,8 @@
       <c r="B43" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="3">
         <v>1</v>
       </c>
@@ -2935,11 +2976,11 @@
       <c r="J43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="34"/>
+      <c r="K43" s="36"/>
       <c r="L43" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M43" s="34"/>
+      <c r="M43" s="36"/>
       <c r="N43" s="19" t="s">
         <v>96</v>
       </c>
@@ -2948,8 +2989,8 @@
       <c r="B44" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="3">
         <v>1000</v>
       </c>
@@ -2968,11 +3009,11 @@
       <c r="J44" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K44" s="34"/>
+      <c r="K44" s="36"/>
       <c r="L44" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M44" s="34"/>
+      <c r="M44" s="36"/>
       <c r="N44" s="19" t="s">
         <v>96</v>
       </c>
@@ -2981,8 +3022,8 @@
       <c r="B45" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="3">
         <v>1234.3209999999999</v>
       </c>
@@ -3001,11 +3042,11 @@
       <c r="J45" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K45" s="34"/>
+      <c r="K45" s="36"/>
       <c r="L45" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M45" s="34"/>
+      <c r="M45" s="36"/>
       <c r="N45" s="19" t="s">
         <v>96</v>
       </c>
@@ -3014,8 +3055,8 @@
       <c r="B46" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="19" t="s">
         <v>101</v>
       </c>
@@ -3034,11 +3075,11 @@
       <c r="J46" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K46" s="34"/>
+      <c r="K46" s="36"/>
       <c r="L46" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M46" s="34"/>
+      <c r="M46" s="36"/>
       <c r="N46" s="19" t="s">
         <v>96</v>
       </c>
@@ -3056,10 +3097,10 @@
       <c r="B48" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D48" s="37" t="s">
         <v>18</v>
       </c>
       <c r="E48" s="3">
@@ -3080,13 +3121,13 @@
       <c r="J48" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K48" s="34" t="s">
+      <c r="K48" s="36" t="s">
         <v>147</v>
       </c>
       <c r="L48" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M48" s="34" t="s">
+      <c r="M48" s="36" t="s">
         <v>147</v>
       </c>
       <c r="N48" s="19" t="s">
@@ -3097,8 +3138,8 @@
       <c r="B49" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="32"/>
-      <c r="D49" s="36"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="37"/>
       <c r="E49" s="3">
         <v>0.5</v>
       </c>
@@ -3117,11 +3158,11 @@
       <c r="J49" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K49" s="35"/>
+      <c r="K49" s="40"/>
       <c r="L49" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M49" s="35"/>
+      <c r="M49" s="40"/>
       <c r="N49" s="19" t="s">
         <v>96</v>
       </c>
@@ -3130,8 +3171,8 @@
       <c r="B50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="36"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="3">
         <v>1</v>
       </c>
@@ -3150,11 +3191,11 @@
       <c r="J50" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K50" s="35"/>
+      <c r="K50" s="40"/>
       <c r="L50" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M50" s="35"/>
+      <c r="M50" s="40"/>
       <c r="N50" s="19" t="s">
         <v>96</v>
       </c>
@@ -3163,8 +3204,8 @@
       <c r="B51" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="32"/>
-      <c r="D51" s="36"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="3">
         <v>0.75</v>
       </c>
@@ -3183,11 +3224,11 @@
       <c r="J51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K51" s="35"/>
+      <c r="K51" s="40"/>
       <c r="L51" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M51" s="35"/>
+      <c r="M51" s="40"/>
       <c r="N51" s="19" t="s">
         <v>96</v>
       </c>
@@ -3196,8 +3237,8 @@
       <c r="B52" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="32"/>
-      <c r="D52" s="36"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="19" t="s">
         <v>108</v>
       </c>
@@ -3216,24 +3257,24 @@
       <c r="J52" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K52" s="35"/>
+      <c r="K52" s="40"/>
       <c r="L52" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M52" s="35"/>
+      <c r="M52" s="40"/>
       <c r="N52" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="2:14" s="39" customFormat="1"/>
+    <row r="53" spans="2:14" s="34" customFormat="1"/>
     <row r="54" spans="2:14" ht="14.4" customHeight="1">
       <c r="B54" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D54" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="19" t="s">
@@ -3254,13 +3295,13 @@
       <c r="J54" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K54" s="31" t="s">
+      <c r="K54" s="41" t="s">
         <v>139</v>
       </c>
       <c r="L54" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M54" s="31" t="s">
+      <c r="M54" s="41" t="s">
         <v>139</v>
       </c>
       <c r="N54" s="19" t="s">
@@ -3271,8 +3312,8 @@
       <c r="B55" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="19" t="s">
         <v>113</v>
       </c>
@@ -3291,11 +3332,11 @@
       <c r="J55" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="31"/>
+      <c r="K55" s="41"/>
       <c r="L55" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M55" s="31"/>
+      <c r="M55" s="41"/>
       <c r="N55" s="19" t="s">
         <v>96</v>
       </c>
@@ -3304,8 +3345,8 @@
       <c r="B56" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="19" t="s">
         <v>115</v>
       </c>
@@ -3324,11 +3365,11 @@
       <c r="J56" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K56" s="31"/>
+      <c r="K56" s="41"/>
       <c r="L56" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M56" s="31"/>
+      <c r="M56" s="41"/>
       <c r="N56" s="19" t="s">
         <v>96</v>
       </c>
@@ -3337,8 +3378,8 @@
       <c r="B57" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="19" t="s">
         <v>117</v>
       </c>
@@ -3357,11 +3398,11 @@
       <c r="J57" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="K57" s="31"/>
+      <c r="K57" s="41"/>
       <c r="L57" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M57" s="31"/>
+      <c r="M57" s="41"/>
       <c r="N57" s="19" t="s">
         <v>96</v>
       </c>
@@ -3370,8 +3411,8 @@
       <c r="B58" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="19" t="s">
         <v>120</v>
       </c>
@@ -3390,11 +3431,11 @@
       <c r="J58" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K58" s="31"/>
+      <c r="K58" s="41"/>
       <c r="L58" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M58" s="31"/>
+      <c r="M58" s="41"/>
       <c r="N58" s="19" t="s">
         <v>96</v>
       </c>
@@ -3403,8 +3444,8 @@
       <c r="B59" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="19" t="s">
         <v>122</v>
       </c>
@@ -3423,11 +3464,11 @@
       <c r="J59" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K59" s="31"/>
+      <c r="K59" s="41"/>
       <c r="L59" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M59" s="31"/>
+      <c r="M59" s="41"/>
       <c r="N59" s="19" t="s">
         <v>96</v>
       </c>
@@ -3435,10 +3476,10 @@
     <row r="60" spans="2:14" s="26" customFormat="1"/>
     <row r="61" spans="2:14" s="25" customFormat="1" ht="14.4" customHeight="1">
       <c r="B61" s="11"/>
-      <c r="C61" s="37" t="s">
+      <c r="C61" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="37" t="s">
+      <c r="D61" s="39" t="s">
         <v>133</v>
       </c>
       <c r="E61" s="23" t="s">
@@ -3459,11 +3500,17 @@
       <c r="J61" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="M61" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="N61" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="62" spans="2:14" s="25" customFormat="1">
       <c r="B62" s="11"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
       <c r="E62" s="23" t="s">
         <v>126</v>
       </c>
@@ -3482,11 +3529,17 @@
       <c r="J62" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="M62" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="N62" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="63" spans="2:14" s="25" customFormat="1">
       <c r="B63" s="11"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
       <c r="E63" s="23" t="s">
         <v>127</v>
       </c>
@@ -3505,11 +3558,17 @@
       <c r="J63" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="M63" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="N63" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="64" spans="2:14" s="25" customFormat="1">
       <c r="B64" s="11"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
       <c r="E64" s="23" t="s">
         <v>128</v>
       </c>
@@ -3528,11 +3587,17 @@
       <c r="J64" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="M64" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="N64" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="65" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B65" s="11"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
       <c r="E65" s="23" t="s">
         <v>129</v>
       </c>
@@ -3551,11 +3616,17 @@
       <c r="J65" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="M65" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="N65" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="66" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B66" s="11"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
       <c r="E66" s="23" t="s">
         <v>130</v>
       </c>
@@ -3574,11 +3645,17 @@
       <c r="J66" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="M66" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="N66" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="67" spans="2:14" s="25" customFormat="1" ht="43.2">
       <c r="B67" s="11"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
       <c r="E67" s="23" t="s">
         <v>131</v>
       </c>
@@ -3597,15 +3674,21 @@
       <c r="J67" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="M67" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="N67" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="68" spans="2:14" s="25" customFormat="1">
       <c r="B68" s="11"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
       <c r="E68" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F68" s="23" t="s">
+      <c r="F68" s="43" t="s">
         <v>91</v>
       </c>
       <c r="G68" s="19" t="s">
@@ -3620,13 +3703,19 @@
       <c r="J68" s="19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="69" spans="2:14" s="38" customFormat="1"/>
+      <c r="M68" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="N68" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" s="42" customFormat="1"/>
     <row r="70" spans="2:14" ht="14.4" customHeight="1">
-      <c r="C70" s="37" t="s">
+      <c r="C70" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="D70" s="37" t="s">
+      <c r="D70" s="39" t="s">
         <v>132</v>
       </c>
       <c r="E70" s="23" t="s">
@@ -3661,8 +3750,8 @@
       </c>
     </row>
     <row r="71" spans="2:14">
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
       <c r="E71" s="23" t="s">
         <v>126</v>
       </c>
@@ -3695,8 +3784,8 @@
       </c>
     </row>
     <row r="72" spans="2:14">
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
       <c r="E72" s="23" t="s">
         <v>127</v>
       </c>
@@ -3729,8 +3818,8 @@
       </c>
     </row>
     <row r="73" spans="2:14" ht="57.6">
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
       <c r="E73" s="23" t="s">
         <v>128</v>
       </c>
@@ -3755,7 +3844,7 @@
       <c r="L73" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M73" s="23" t="s">
+      <c r="M73" s="43" t="s">
         <v>134</v>
       </c>
       <c r="N73" s="10" t="s">
@@ -3763,8 +3852,8 @@
       </c>
     </row>
     <row r="74" spans="2:14" ht="28.8">
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="39"/>
       <c r="E74" s="23" t="s">
         <v>129</v>
       </c>
@@ -3789,7 +3878,7 @@
       <c r="L74" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M74" s="42" t="s">
+      <c r="M74" s="31" t="s">
         <v>146</v>
       </c>
       <c r="N74" s="13" t="s">
@@ -3797,8 +3886,8 @@
       </c>
     </row>
     <row r="75" spans="2:14" ht="28.8">
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
       <c r="E75" s="23" t="s">
         <v>130</v>
       </c>
@@ -3823,7 +3912,7 @@
       <c r="L75" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M75" s="42" t="s">
+      <c r="M75" s="31" t="s">
         <v>146</v>
       </c>
       <c r="N75" s="13" t="s">
@@ -3831,8 +3920,8 @@
       </c>
     </row>
     <row r="76" spans="2:14" ht="43.2">
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="39"/>
       <c r="E76" s="23" t="s">
         <v>131</v>
       </c>
@@ -3857,7 +3946,7 @@
       <c r="L76" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M76" s="42" t="s">
+      <c r="M76" s="31" t="s">
         <v>149</v>
       </c>
       <c r="N76" s="13" t="s">
@@ -3865,8 +3954,8 @@
       </c>
     </row>
     <row r="77" spans="2:14">
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="39"/>
       <c r="E77" s="23" t="s">
         <v>51</v>
       </c>
@@ -3908,14 +3997,20 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="M9:M14"/>
+    <mergeCell ref="C70:C77"/>
+    <mergeCell ref="D70:D77"/>
+    <mergeCell ref="A69:XFD69"/>
+    <mergeCell ref="M54:M59"/>
+    <mergeCell ref="K16:K25"/>
+    <mergeCell ref="K54:K59"/>
+    <mergeCell ref="K42:K46"/>
+    <mergeCell ref="K48:K52"/>
+    <mergeCell ref="C16:C25"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="C61:C68"/>
+    <mergeCell ref="D61:D68"/>
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="C54:C59"/>
     <mergeCell ref="D4:D7"/>
@@ -3932,24 +4027,18 @@
     <mergeCell ref="M16:M25"/>
     <mergeCell ref="M42:M46"/>
     <mergeCell ref="M48:M52"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="A15:XFD15"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="M9:M14"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C16:C25"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="C61:C68"/>
-    <mergeCell ref="D61:D68"/>
-    <mergeCell ref="C70:C77"/>
-    <mergeCell ref="D70:D77"/>
-    <mergeCell ref="A69:XFD69"/>
-    <mergeCell ref="M54:M59"/>
-    <mergeCell ref="K16:K25"/>
-    <mergeCell ref="K54:K59"/>
     <mergeCell ref="K4:K7"/>
     <mergeCell ref="K9:K14"/>
-    <mergeCell ref="K42:K46"/>
-    <mergeCell ref="K48:K52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update Traceability Matrix Report for MS5
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
+++ b/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zohrab Zeynalli\OneDrive\Documents\SENECA\2semester\SFT221\SFT221_GROUP_PROJECT\Documents\Testing\TestsDocuments\ms5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\MS5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41615D93-993D-4F72-9F6F-D1F7EAEB9E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60109145-7317-4B08-974E-F401E0E72C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1015,12 +1015,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1254,7 +1261,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1270,122 +1277,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1665,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" topLeftCell="G66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1706,22 +1713,22 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="32" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="32" t="s">
+      <c r="J2" s="42"/>
+      <c r="K2" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="32" t="s">
+      <c r="L2" s="42"/>
+      <c r="M2" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="33"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="1:14" ht="29.4" thickBot="1">
       <c r="A3" s="5" t="s">
@@ -1769,10 +1776,10 @@
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="39" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3">
@@ -1793,13 +1800,13 @@
       <c r="J4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="43" t="s">
         <v>147</v>
       </c>
       <c r="N4" s="19" t="s">
@@ -1810,8 +1817,8 @@
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="3">
         <v>1000</v>
       </c>
@@ -1830,11 +1837,11 @@
       <c r="J5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="36"/>
+      <c r="K5" s="37"/>
       <c r="L5" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="36"/>
+      <c r="M5" s="37"/>
       <c r="N5" s="19" t="s">
         <v>96</v>
       </c>
@@ -1843,8 +1850,8 @@
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="37"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="3">
         <v>-0.1</v>
       </c>
@@ -1863,11 +1870,11 @@
       <c r="J6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="36"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M6" s="36"/>
+      <c r="M6" s="37"/>
       <c r="N6" s="19" t="s">
         <v>96</v>
       </c>
@@ -1876,8 +1883,8 @@
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="37"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="3">
         <v>1000.1</v>
       </c>
@@ -1896,24 +1903,24 @@
       <c r="J7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="36"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M7" s="36"/>
+      <c r="M7" s="37"/>
       <c r="N7" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="34" customFormat="1"/>
+    <row r="8" spans="1:14" s="40" customFormat="1"/>
     <row r="9" spans="1:14" ht="43.2" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="39" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="3">
@@ -1934,13 +1941,13 @@
       <c r="J9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="37" t="s">
         <v>147</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="M9" s="37" t="s">
         <v>147</v>
       </c>
       <c r="N9" s="19" t="s">
@@ -1951,8 +1958,8 @@
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="3">
         <v>0.5</v>
       </c>
@@ -1971,11 +1978,11 @@
       <c r="J10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="36"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="36"/>
+      <c r="M10" s="37"/>
       <c r="N10" s="19" t="s">
         <v>96</v>
       </c>
@@ -1984,8 +1991,8 @@
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="37"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="3">
         <v>1</v>
       </c>
@@ -2004,11 +2011,11 @@
       <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="36"/>
+      <c r="K11" s="37"/>
       <c r="L11" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M11" s="36"/>
+      <c r="M11" s="37"/>
       <c r="N11" s="19" t="s">
         <v>96</v>
       </c>
@@ -2017,8 +2024,8 @@
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="37"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="3">
         <v>0.24</v>
       </c>
@@ -2037,11 +2044,11 @@
       <c r="J12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="36"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M12" s="36"/>
+      <c r="M12" s="37"/>
       <c r="N12" s="19" t="s">
         <v>96</v>
       </c>
@@ -2050,8 +2057,8 @@
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="37"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="3">
         <v>-0.5</v>
       </c>
@@ -2070,11 +2077,11 @@
       <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M13" s="36"/>
+      <c r="M13" s="37"/>
       <c r="N13" s="19" t="s">
         <v>96</v>
       </c>
@@ -2083,8 +2090,8 @@
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="37"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -2103,24 +2110,24 @@
       <c r="J14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="36"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M14" s="36"/>
+      <c r="M14" s="37"/>
       <c r="N14" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="34" customFormat="1"/>
+    <row r="15" spans="1:14" s="40" customFormat="1"/>
     <row r="16" spans="1:14">
       <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="33" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2141,13 +2148,13 @@
       <c r="J16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="41" t="s">
+      <c r="K16" s="35" t="s">
         <v>139</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M16" s="41" t="s">
+      <c r="M16" s="35" t="s">
         <v>139</v>
       </c>
       <c r="N16" s="19" t="s">
@@ -2158,8 +2165,8 @@
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
@@ -2178,11 +2185,11 @@
       <c r="J17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="38"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M17" s="38"/>
+      <c r="M17" s="36"/>
       <c r="N17" s="19" t="s">
         <v>96</v>
       </c>
@@ -2191,8 +2198,8 @@
       <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="3" t="s">
         <v>32</v>
       </c>
@@ -2211,11 +2218,11 @@
       <c r="J18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="38"/>
+      <c r="K18" s="36"/>
       <c r="L18" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M18" s="38"/>
+      <c r="M18" s="36"/>
       <c r="N18" s="19" t="s">
         <v>96</v>
       </c>
@@ -2224,8 +2231,8 @@
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="3" t="s">
         <v>34</v>
       </c>
@@ -2244,11 +2251,11 @@
       <c r="J19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="38"/>
+      <c r="K19" s="36"/>
       <c r="L19" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M19" s="38"/>
+      <c r="M19" s="36"/>
       <c r="N19" s="19" t="s">
         <v>96</v>
       </c>
@@ -2257,8 +2264,8 @@
       <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2277,11 +2284,11 @@
       <c r="J20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="38"/>
+      <c r="K20" s="36"/>
       <c r="L20" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M20" s="38"/>
+      <c r="M20" s="36"/>
       <c r="N20" s="19" t="s">
         <v>96</v>
       </c>
@@ -2290,8 +2297,8 @@
       <c r="B21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="3" t="s">
         <v>38</v>
       </c>
@@ -2310,11 +2317,11 @@
       <c r="J21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="38"/>
+      <c r="K21" s="36"/>
       <c r="L21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M21" s="38"/>
+      <c r="M21" s="36"/>
       <c r="N21" s="19" t="s">
         <v>96</v>
       </c>
@@ -2323,8 +2330,8 @@
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
@@ -2343,11 +2350,11 @@
       <c r="J22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="38"/>
+      <c r="K22" s="36"/>
       <c r="L22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M22" s="38"/>
+      <c r="M22" s="36"/>
       <c r="N22" s="19" t="s">
         <v>96</v>
       </c>
@@ -2356,8 +2363,8 @@
       <c r="B23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="3" t="s">
         <v>42</v>
       </c>
@@ -2376,11 +2383,11 @@
       <c r="J23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="38"/>
+      <c r="K23" s="36"/>
       <c r="L23" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M23" s="38"/>
+      <c r="M23" s="36"/>
       <c r="N23" s="19" t="s">
         <v>96</v>
       </c>
@@ -2389,8 +2396,8 @@
       <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="3" t="s">
         <v>44</v>
       </c>
@@ -2409,11 +2416,11 @@
       <c r="J24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="38"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M24" s="38"/>
+      <c r="M24" s="36"/>
       <c r="N24" s="19" t="s">
         <v>96</v>
       </c>
@@ -2422,8 +2429,8 @@
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="3" t="s">
         <v>47</v>
       </c>
@@ -2442,24 +2449,24 @@
       <c r="J25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="38"/>
+      <c r="K25" s="36"/>
       <c r="L25" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M25" s="38"/>
+      <c r="M25" s="36"/>
       <c r="N25" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="2:14" s="34" customFormat="1"/>
+    <row r="26" spans="2:14" s="40" customFormat="1"/>
     <row r="27" spans="2:14" ht="28.8" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="39" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -2497,8 +2504,8 @@
       <c r="B28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="37"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="39"/>
       <c r="E28" s="3" t="s">
         <v>78</v>
       </c>
@@ -2534,8 +2541,8 @@
       <c r="B29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="37"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="3" t="s">
         <v>61</v>
       </c>
@@ -2571,8 +2578,8 @@
       <c r="B30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="37"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="39"/>
       <c r="E30" s="3" t="s">
         <v>64</v>
       </c>
@@ -2608,8 +2615,8 @@
       <c r="B31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="37"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="39"/>
       <c r="E31" s="3" t="s">
         <v>68</v>
       </c>
@@ -2645,8 +2652,8 @@
       <c r="B32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="38"/>
-      <c r="D32" s="37"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="39"/>
       <c r="E32" s="14" t="s">
         <v>71</v>
       </c>
@@ -2682,8 +2689,8 @@
       <c r="B33" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="37"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="39"/>
       <c r="E33" s="3" t="s">
         <v>74</v>
       </c>
@@ -2719,8 +2726,8 @@
       <c r="B34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="37"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="39"/>
       <c r="E34" s="3" t="s">
         <v>56</v>
       </c>
@@ -2756,8 +2763,8 @@
       <c r="B35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="37"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="39"/>
       <c r="E35" s="3" t="s">
         <v>80</v>
       </c>
@@ -2793,8 +2800,8 @@
       <c r="B36" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="37"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="39"/>
       <c r="E36" s="15" t="s">
         <v>82</v>
       </c>
@@ -2826,7 +2833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:14" s="34" customFormat="1"/>
+    <row r="37" spans="2:14" s="40" customFormat="1"/>
     <row r="38" spans="2:14" ht="43.2">
       <c r="B38" s="6" t="s">
         <v>83</v>
@@ -2868,7 +2875,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:14" s="34" customFormat="1"/>
+    <row r="39" spans="2:14" s="40" customFormat="1"/>
     <row r="40" spans="2:14" ht="15" customHeight="1">
       <c r="B40" s="6" t="s">
         <v>88</v>
@@ -2910,15 +2917,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:14" s="34" customFormat="1"/>
+    <row r="41" spans="2:14" s="40" customFormat="1"/>
     <row r="42" spans="2:14" ht="14.4" customHeight="1">
       <c r="B42" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D42" s="39" t="s">
         <v>95</v>
       </c>
       <c r="E42" s="3">
@@ -2939,13 +2946,13 @@
       <c r="J42" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K42" s="36" t="s">
+      <c r="K42" s="37" t="s">
         <v>147</v>
       </c>
       <c r="L42" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M42" s="36" t="s">
+      <c r="M42" s="37" t="s">
         <v>147</v>
       </c>
       <c r="N42" s="19" t="s">
@@ -2956,8 +2963,8 @@
       <c r="B43" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
       <c r="E43" s="3">
         <v>1</v>
       </c>
@@ -2976,11 +2983,11 @@
       <c r="J43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="36"/>
+      <c r="K43" s="37"/>
       <c r="L43" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M43" s="36"/>
+      <c r="M43" s="37"/>
       <c r="N43" s="19" t="s">
         <v>96</v>
       </c>
@@ -2989,8 +2996,8 @@
       <c r="B44" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
       <c r="E44" s="3">
         <v>1000</v>
       </c>
@@ -3009,11 +3016,11 @@
       <c r="J44" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K44" s="36"/>
+      <c r="K44" s="37"/>
       <c r="L44" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M44" s="36"/>
+      <c r="M44" s="37"/>
       <c r="N44" s="19" t="s">
         <v>96</v>
       </c>
@@ -3022,8 +3029,8 @@
       <c r="B45" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
       <c r="E45" s="3">
         <v>1234.3209999999999</v>
       </c>
@@ -3042,11 +3049,11 @@
       <c r="J45" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K45" s="36"/>
+      <c r="K45" s="37"/>
       <c r="L45" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M45" s="36"/>
+      <c r="M45" s="37"/>
       <c r="N45" s="19" t="s">
         <v>96</v>
       </c>
@@ -3055,8 +3062,8 @@
       <c r="B46" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
       <c r="E46" s="19" t="s">
         <v>101</v>
       </c>
@@ -3075,11 +3082,11 @@
       <c r="J46" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K46" s="36"/>
+      <c r="K46" s="37"/>
       <c r="L46" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M46" s="36"/>
+      <c r="M46" s="37"/>
       <c r="N46" s="19" t="s">
         <v>96</v>
       </c>
@@ -3097,10 +3104,10 @@
       <c r="B48" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C48" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="39" t="s">
         <v>18</v>
       </c>
       <c r="E48" s="3">
@@ -3121,13 +3128,13 @@
       <c r="J48" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K48" s="36" t="s">
+      <c r="K48" s="37" t="s">
         <v>147</v>
       </c>
       <c r="L48" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M48" s="36" t="s">
+      <c r="M48" s="37" t="s">
         <v>147</v>
       </c>
       <c r="N48" s="19" t="s">
@@ -3138,8 +3145,8 @@
       <c r="B49" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="38"/>
-      <c r="D49" s="37"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="39"/>
       <c r="E49" s="3">
         <v>0.5</v>
       </c>
@@ -3158,11 +3165,11 @@
       <c r="J49" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K49" s="40"/>
+      <c r="K49" s="38"/>
       <c r="L49" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M49" s="40"/>
+      <c r="M49" s="38"/>
       <c r="N49" s="19" t="s">
         <v>96</v>
       </c>
@@ -3171,8 +3178,8 @@
       <c r="B50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="38"/>
-      <c r="D50" s="37"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="39"/>
       <c r="E50" s="3">
         <v>1</v>
       </c>
@@ -3191,11 +3198,11 @@
       <c r="J50" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K50" s="40"/>
+      <c r="K50" s="38"/>
       <c r="L50" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M50" s="40"/>
+      <c r="M50" s="38"/>
       <c r="N50" s="19" t="s">
         <v>96</v>
       </c>
@@ -3204,8 +3211,8 @@
       <c r="B51" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="38"/>
-      <c r="D51" s="37"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="39"/>
       <c r="E51" s="3">
         <v>0.75</v>
       </c>
@@ -3224,11 +3231,11 @@
       <c r="J51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K51" s="40"/>
+      <c r="K51" s="38"/>
       <c r="L51" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M51" s="40"/>
+      <c r="M51" s="38"/>
       <c r="N51" s="19" t="s">
         <v>96</v>
       </c>
@@ -3237,8 +3244,8 @@
       <c r="B52" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="38"/>
-      <c r="D52" s="37"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="39"/>
       <c r="E52" s="19" t="s">
         <v>108</v>
       </c>
@@ -3257,24 +3264,24 @@
       <c r="J52" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K52" s="40"/>
+      <c r="K52" s="38"/>
       <c r="L52" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M52" s="40"/>
+      <c r="M52" s="38"/>
       <c r="N52" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="2:14" s="34" customFormat="1"/>
+    <row r="53" spans="2:14" s="40" customFormat="1"/>
     <row r="54" spans="2:14" ht="14.4" customHeight="1">
       <c r="B54" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="37" t="s">
+      <c r="C54" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="39" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="19" t="s">
@@ -3295,13 +3302,13 @@
       <c r="J54" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K54" s="41" t="s">
+      <c r="K54" s="35" t="s">
         <v>139</v>
       </c>
       <c r="L54" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M54" s="41" t="s">
+      <c r="M54" s="35" t="s">
         <v>139</v>
       </c>
       <c r="N54" s="19" t="s">
@@ -3312,8 +3319,8 @@
       <c r="B55" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
       <c r="E55" s="19" t="s">
         <v>113</v>
       </c>
@@ -3332,11 +3339,11 @@
       <c r="J55" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="41"/>
+      <c r="K55" s="35"/>
       <c r="L55" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M55" s="41"/>
+      <c r="M55" s="35"/>
       <c r="N55" s="19" t="s">
         <v>96</v>
       </c>
@@ -3345,8 +3352,8 @@
       <c r="B56" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
       <c r="E56" s="19" t="s">
         <v>115</v>
       </c>
@@ -3365,11 +3372,11 @@
       <c r="J56" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K56" s="41"/>
+      <c r="K56" s="35"/>
       <c r="L56" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M56" s="41"/>
+      <c r="M56" s="35"/>
       <c r="N56" s="19" t="s">
         <v>96</v>
       </c>
@@ -3378,8 +3385,8 @@
       <c r="B57" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
       <c r="E57" s="19" t="s">
         <v>117</v>
       </c>
@@ -3398,11 +3405,11 @@
       <c r="J57" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="K57" s="41"/>
+      <c r="K57" s="35"/>
       <c r="L57" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M57" s="41"/>
+      <c r="M57" s="35"/>
       <c r="N57" s="19" t="s">
         <v>96</v>
       </c>
@@ -3411,8 +3418,8 @@
       <c r="B58" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
       <c r="E58" s="19" t="s">
         <v>120</v>
       </c>
@@ -3431,11 +3438,11 @@
       <c r="J58" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K58" s="41"/>
+      <c r="K58" s="35"/>
       <c r="L58" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M58" s="41"/>
+      <c r="M58" s="35"/>
       <c r="N58" s="19" t="s">
         <v>96</v>
       </c>
@@ -3444,8 +3451,8 @@
       <c r="B59" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
       <c r="E59" s="19" t="s">
         <v>122</v>
       </c>
@@ -3464,11 +3471,11 @@
       <c r="J59" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K59" s="41"/>
+      <c r="K59" s="35"/>
       <c r="L59" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M59" s="41"/>
+      <c r="M59" s="35"/>
       <c r="N59" s="19" t="s">
         <v>96</v>
       </c>
@@ -3476,10 +3483,10 @@
     <row r="60" spans="2:14" s="26" customFormat="1"/>
     <row r="61" spans="2:14" s="25" customFormat="1" ht="14.4" customHeight="1">
       <c r="B61" s="11"/>
-      <c r="C61" s="39" t="s">
+      <c r="C61" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="39" t="s">
+      <c r="D61" s="33" t="s">
         <v>133</v>
       </c>
       <c r="E61" s="23" t="s">
@@ -3509,8 +3516,8 @@
     </row>
     <row r="62" spans="2:14" s="25" customFormat="1">
       <c r="B62" s="11"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
       <c r="E62" s="23" t="s">
         <v>126</v>
       </c>
@@ -3538,8 +3545,8 @@
     </row>
     <row r="63" spans="2:14" s="25" customFormat="1">
       <c r="B63" s="11"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
       <c r="E63" s="23" t="s">
         <v>127</v>
       </c>
@@ -3567,8 +3574,8 @@
     </row>
     <row r="64" spans="2:14" s="25" customFormat="1">
       <c r="B64" s="11"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
       <c r="E64" s="23" t="s">
         <v>128</v>
       </c>
@@ -3596,8 +3603,8 @@
     </row>
     <row r="65" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B65" s="11"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
       <c r="E65" s="23" t="s">
         <v>129</v>
       </c>
@@ -3625,8 +3632,8 @@
     </row>
     <row r="66" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B66" s="11"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="33"/>
       <c r="E66" s="23" t="s">
         <v>130</v>
       </c>
@@ -3654,8 +3661,8 @@
     </row>
     <row r="67" spans="2:14" s="25" customFormat="1" ht="43.2">
       <c r="B67" s="11"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
       <c r="E67" s="23" t="s">
         <v>131</v>
       </c>
@@ -3683,12 +3690,12 @@
     </row>
     <row r="68" spans="2:14" s="25" customFormat="1">
       <c r="B68" s="11"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
       <c r="E68" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F68" s="43" t="s">
+      <c r="F68" s="32" t="s">
         <v>91</v>
       </c>
       <c r="G68" s="19" t="s">
@@ -3710,12 +3717,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="2:14" s="42" customFormat="1"/>
+    <row r="69" spans="2:14" s="34" customFormat="1"/>
     <row r="70" spans="2:14" ht="14.4" customHeight="1">
-      <c r="C70" s="39" t="s">
+      <c r="C70" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="D70" s="39" t="s">
+      <c r="D70" s="33" t="s">
         <v>132</v>
       </c>
       <c r="E70" s="23" t="s">
@@ -3739,19 +3746,19 @@
       <c r="K70" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L70" s="13" t="s">
-        <v>30</v>
+      <c r="L70" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="M70" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="N70" s="13" t="s">
-        <v>30</v>
+      <c r="N70" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="2:14">
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
       <c r="E71" s="23" t="s">
         <v>126</v>
       </c>
@@ -3784,8 +3791,8 @@
       </c>
     </row>
     <row r="72" spans="2:14">
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
       <c r="E72" s="23" t="s">
         <v>127</v>
       </c>
@@ -3818,8 +3825,8 @@
       </c>
     </row>
     <row r="73" spans="2:14" ht="57.6">
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
       <c r="E73" s="23" t="s">
         <v>128</v>
       </c>
@@ -3844,7 +3851,7 @@
       <c r="L73" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M73" s="43" t="s">
+      <c r="M73" s="32" t="s">
         <v>134</v>
       </c>
       <c r="N73" s="10" t="s">
@@ -3852,8 +3859,8 @@
       </c>
     </row>
     <row r="74" spans="2:14" ht="28.8">
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
       <c r="E74" s="23" t="s">
         <v>129</v>
       </c>
@@ -3886,8 +3893,8 @@
       </c>
     </row>
     <row r="75" spans="2:14" ht="28.8">
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="33"/>
       <c r="E75" s="23" t="s">
         <v>130</v>
       </c>
@@ -3920,8 +3927,8 @@
       </c>
     </row>
     <row r="76" spans="2:14" ht="43.2">
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
       <c r="E76" s="23" t="s">
         <v>131</v>
       </c>
@@ -3954,8 +3961,8 @@
       </c>
     </row>
     <row r="77" spans="2:14">
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
       <c r="E77" s="23" t="s">
         <v>51</v>
       </c>
@@ -3997,6 +4004,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A53:XFD53"/>
+    <mergeCell ref="M16:M25"/>
+    <mergeCell ref="M42:M46"/>
+    <mergeCell ref="M48:M52"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="A15:XFD15"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="M9:M14"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K9:K14"/>
+    <mergeCell ref="D48:D52"/>
+    <mergeCell ref="A26:XFD26"/>
+    <mergeCell ref="A37:XFD37"/>
+    <mergeCell ref="A39:XFD39"/>
+    <mergeCell ref="A41:XFD41"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="D16:D25"/>
+    <mergeCell ref="D27:D36"/>
+    <mergeCell ref="D42:D46"/>
     <mergeCell ref="C70:C77"/>
     <mergeCell ref="D70:D77"/>
     <mergeCell ref="A69:XFD69"/>
@@ -4013,32 +4046,6 @@
     <mergeCell ref="D61:D68"/>
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="D16:D25"/>
-    <mergeCell ref="D27:D36"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="A26:XFD26"/>
-    <mergeCell ref="A37:XFD37"/>
-    <mergeCell ref="A39:XFD39"/>
-    <mergeCell ref="A41:XFD41"/>
-    <mergeCell ref="A53:XFD53"/>
-    <mergeCell ref="M16:M25"/>
-    <mergeCell ref="M42:M46"/>
-    <mergeCell ref="M48:M52"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="M9:M14"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K9:K14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update revised version of Traceablility Matrix for MS5
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
+++ b/Documents/Testing/TestsDocuments/ms5/ms5-traceability-matrix-group5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zohrab Zeynalli\OneDrive\Documents\SENECA\2semester\SFT221\SFT221_GROUP_PROJECT\Documents\Testing\TestsDocuments\ms5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Chan\Desktop\Seneca-Summer-2023\SFT221\Milestone Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26FE4FD-F881-49AD-BF5D-BF622D3E355E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32C24B8-0EA1-4B00-95F4-E703C992F020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="164">
   <si>
     <t>Business Requirements</t>
   </si>
@@ -71,7 +71,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Black-box:</t>
@@ -81,7 +81,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -94,7 +94,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Linking the function </t>
@@ -105,7 +105,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>validatePackageWeight()</t>
@@ -115,7 +115,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> to unit test and
@@ -127,7 +127,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>assert (AreEqual)</t>
@@ -137,7 +137,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> for testing. 
@@ -166,7 +166,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Black-box:</t>
@@ -176,7 +176,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -189,7 +189,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Linking the function
@@ -201,7 +201,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> validatePackageBox()</t>
@@ -211,7 +211,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">  to unit test and
@@ -223,7 +223,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> assert (AreEqual)</t>
@@ -233,7 +233,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> for testing. 
@@ -265,7 +265,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Black-box:</t>
@@ -275,7 +275,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -288,7 +288,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Linking the function
@@ -300,7 +300,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>validateDestination()</t>
@@ -310,7 +310,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">  to unit test and
@@ -322,7 +322,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>assert (AreEqual)</t>
@@ -332,7 +332,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> for testing. 
@@ -414,7 +414,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Pass the data using user input in the </t>
@@ -425,7 +425,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>console</t>
@@ -435,7 +435,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> and capture the result.
@@ -581,7 +581,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>White-box:</t>
@@ -591,7 +591,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -604,7 +604,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Linking the function </t>
@@ -615,7 +615,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>validatePackageWeight()</t>
@@ -625,7 +625,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> to unit test and
@@ -661,7 +661,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>White-box:</t>
@@ -671,7 +671,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -703,7 +703,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>White-box:</t>
@@ -713,7 +713,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -773,7 +773,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -860,10 +860,6 @@
 7T, 7U, 7V, 7W, 7X, 7Y, 8Y</t>
   </si>
   <si>
-    <t>Ship on BLUE LINE, divert 18V, 17V, 16V, 15V, 14V, 13V, 12V, 11V, 10V, 9V, 
-8V, 7V, 7W, 7X, 7Y, 8Y</t>
-  </si>
-  <si>
     <t>Invalid destination format</t>
   </si>
   <si>
@@ -953,15 +949,152 @@
     <t>Valid message shown</t>
   </si>
   <si>
+    <t xml:space="preserve">              Invalid weight (must be 1-1000 Kg.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       Invalid destination format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Ship on BLUE LINE, no diversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Thanks for shipping with Seneca!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   Invalid size                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">              Ship on GREEN LINE, divert: 8Y, 8Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Ship on GREEN LINE, divert: 8Y, 8Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Thanks for shipping with Seneca!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Invalid destination format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              Invalid size                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Ship on BLUE LINE, divert: 11K, 10K, 10J, 9J, 9I, 8I, 8H, 7H, 7G, 6G, 6F, 5F, 5E, 4E, 4D, 3D, 3C, 2C, 2B, 1B, 1A, 0A, 12L</t>
+  </si>
+  <si>
+    <t>Generate a .c file where the main() method contains the test data. Change the argument list of input function. Within the main() method, call this function and pass the data to it. Compare the actual output with the expected output (sample output).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GREEN LINE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, divert: 
+7T, 7U, 7V, 7W, 7X, 7Y, 8Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ship on</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BLUE LINE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, divert 18V, 17V, 16V, 15V, 14V, 13V, 12V, 11V, 10V, 9V, 
+8V, 7V, 7W, 7X, 7Y, 8Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                 Ship on GREEN LINE, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>divert: 8Y, 8Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                 Ship on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GREEN LINE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>divert: 8Y, 8Y</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">CAPACITY REACHED! Go to next closet Route
 Ship on </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -988,52 +1121,13 @@
       </rPr>
       <t>divert: 8Y, 8Y</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">              Invalid weight (must be 1-1000 Kg.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                       Invalid destination format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                   Ship on BLUE LINE, no diversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 Ship on GREEN LINE, divert: 8Y, 8Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                   Thanks for shipping with Seneca!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                   Invalid size                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">              Ship on GREEN LINE, divert: 8Y, 8Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               Ship on GREEN LINE, divert: 8Y, 8Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               Thanks for shipping with Seneca!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                   Invalid destination format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                              Invalid size                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Ship on BLUE LINE, divert: 11K, 10K, 10J, 9J, 9I, 8I, 8H, 7H, 7G, 6G, 6F, 5F, 5E, 4E, 4D, 3D, 3C, 2C, 2B, 1B, 1A, 0A, 12L</t>
-  </si>
-  <si>
-    <t>Generate a .c file where the main() method contains the test data. Change the argument list of input function. Within the main() method, call this function and pass the data to it. Compare the actual output with the expected output (sample output).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1070,12 +1164,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1083,7 +1184,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1091,14 +1192,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1106,13 +1207,13 @@
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1120,7 +1221,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1128,7 +1229,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1137,7 +1238,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1145,7 +1246,7 @@
       <sz val="11"/>
       <color theme="4"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1184,6 +1285,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1279,9 +1394,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1295,125 +1410,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1693,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61:D68"/>
+    <sheetView tabSelected="1" topLeftCell="E56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M76" sqref="M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1734,22 +1855,22 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="39"/>
+      <c r="I2" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="39"/>
+      <c r="K2" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="39"/>
+      <c r="M2" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="N2" s="42"/>
+      <c r="N2" s="39"/>
     </row>
     <row r="3" spans="1:14" ht="29.4" thickBot="1">
       <c r="A3" s="5" t="s">
@@ -1797,10 +1918,10 @@
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="41" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3">
@@ -1821,14 +1942,14 @@
       <c r="J4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="43" t="s">
-        <v>146</v>
+      <c r="K4" s="40" t="s">
+        <v>145</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M4" s="43" t="s">
-        <v>146</v>
+      <c r="M4" s="40" t="s">
+        <v>145</v>
       </c>
       <c r="N4" s="19" t="s">
         <v>96</v>
@@ -1838,8 +1959,8 @@
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="39"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="41"/>
       <c r="E5" s="3">
         <v>1000</v>
       </c>
@@ -1858,11 +1979,11 @@
       <c r="J5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="36"/>
       <c r="L5" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="37"/>
+      <c r="M5" s="36"/>
       <c r="N5" s="19" t="s">
         <v>96</v>
       </c>
@@ -1871,8 +1992,8 @@
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="39"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="3">
         <v>-0.1</v>
       </c>
@@ -1891,11 +2012,11 @@
       <c r="J6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="36"/>
       <c r="L6" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M6" s="37"/>
+      <c r="M6" s="36"/>
       <c r="N6" s="19" t="s">
         <v>96</v>
       </c>
@@ -1904,8 +2025,8 @@
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="39"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="3">
         <v>1000.1</v>
       </c>
@@ -1924,24 +2045,24 @@
       <c r="J7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="37"/>
+      <c r="K7" s="36"/>
       <c r="L7" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M7" s="37"/>
+      <c r="M7" s="36"/>
       <c r="N7" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="40" customFormat="1"/>
+    <row r="8" spans="1:14" s="33" customFormat="1"/>
     <row r="9" spans="1:14" ht="43.2" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="3">
@@ -1962,14 +2083,14 @@
       <c r="J9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="37" t="s">
-        <v>146</v>
+      <c r="K9" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M9" s="37" t="s">
-        <v>146</v>
+      <c r="M9" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="N9" s="19" t="s">
         <v>96</v>
@@ -1979,8 +2100,8 @@
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="39"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="3">
         <v>0.5</v>
       </c>
@@ -1999,11 +2120,11 @@
       <c r="J10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="36"/>
       <c r="L10" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="37"/>
+      <c r="M10" s="36"/>
       <c r="N10" s="19" t="s">
         <v>96</v>
       </c>
@@ -2012,8 +2133,8 @@
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="3">
         <v>1</v>
       </c>
@@ -2032,11 +2153,11 @@
       <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="37"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M11" s="37"/>
+      <c r="M11" s="36"/>
       <c r="N11" s="19" t="s">
         <v>96</v>
       </c>
@@ -2045,8 +2166,8 @@
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="39"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="3">
         <v>0.24</v>
       </c>
@@ -2065,11 +2186,11 @@
       <c r="J12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="37"/>
+      <c r="K12" s="36"/>
       <c r="L12" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M12" s="37"/>
+      <c r="M12" s="36"/>
       <c r="N12" s="19" t="s">
         <v>96</v>
       </c>
@@ -2078,8 +2199,8 @@
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="39"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="3">
         <v>-0.5</v>
       </c>
@@ -2098,11 +2219,11 @@
       <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="36"/>
       <c r="L13" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M13" s="37"/>
+      <c r="M13" s="36"/>
       <c r="N13" s="19" t="s">
         <v>96</v>
       </c>
@@ -2111,8 +2232,8 @@
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -2131,24 +2252,24 @@
       <c r="J14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="37"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M14" s="37"/>
+      <c r="M14" s="36"/>
       <c r="N14" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="40" customFormat="1"/>
+    <row r="15" spans="1:14" s="33" customFormat="1"/>
     <row r="16" spans="1:14">
       <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="42" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2169,14 +2290,14 @@
       <c r="J16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="35" t="s">
-        <v>138</v>
+      <c r="K16" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M16" s="35" t="s">
-        <v>138</v>
+      <c r="M16" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="N16" s="19" t="s">
         <v>96</v>
@@ -2186,8 +2307,8 @@
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
@@ -2206,11 +2327,11 @@
       <c r="J17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="36"/>
+      <c r="K17" s="35"/>
       <c r="L17" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M17" s="36"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="19" t="s">
         <v>96</v>
       </c>
@@ -2219,8 +2340,8 @@
       <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="3" t="s">
         <v>32</v>
       </c>
@@ -2239,11 +2360,11 @@
       <c r="J18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="36"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M18" s="36"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="19" t="s">
         <v>96</v>
       </c>
@@ -2252,8 +2373,8 @@
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="3" t="s">
         <v>34</v>
       </c>
@@ -2272,11 +2393,11 @@
       <c r="J19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="36"/>
+      <c r="K19" s="35"/>
       <c r="L19" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M19" s="36"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="19" t="s">
         <v>96</v>
       </c>
@@ -2285,8 +2406,8 @@
       <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2305,11 +2426,11 @@
       <c r="J20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="36"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M20" s="36"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="19" t="s">
         <v>96</v>
       </c>
@@ -2318,8 +2439,8 @@
       <c r="B21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="3" t="s">
         <v>38</v>
       </c>
@@ -2338,11 +2459,11 @@
       <c r="J21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="36"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M21" s="36"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="19" t="s">
         <v>96</v>
       </c>
@@ -2351,8 +2472,8 @@
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
@@ -2371,11 +2492,11 @@
       <c r="J22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="36"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M22" s="36"/>
+      <c r="M22" s="35"/>
       <c r="N22" s="19" t="s">
         <v>96</v>
       </c>
@@ -2384,8 +2505,8 @@
       <c r="B23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="3" t="s">
         <v>42</v>
       </c>
@@ -2404,11 +2525,11 @@
       <c r="J23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="36"/>
+      <c r="K23" s="35"/>
       <c r="L23" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M23" s="36"/>
+      <c r="M23" s="35"/>
       <c r="N23" s="19" t="s">
         <v>96</v>
       </c>
@@ -2417,8 +2538,8 @@
       <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="3" t="s">
         <v>44</v>
       </c>
@@ -2437,11 +2558,11 @@
       <c r="J24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="36"/>
+      <c r="K24" s="35"/>
       <c r="L24" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M24" s="36"/>
+      <c r="M24" s="35"/>
       <c r="N24" s="19" t="s">
         <v>96</v>
       </c>
@@ -2450,8 +2571,8 @@
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="3" t="s">
         <v>47</v>
       </c>
@@ -2470,24 +2591,24 @@
       <c r="J25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="36"/>
+      <c r="K25" s="35"/>
       <c r="L25" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M25" s="36"/>
+      <c r="M25" s="35"/>
       <c r="N25" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="2:14" s="40" customFormat="1"/>
+    <row r="26" spans="2:14" s="33" customFormat="1"/>
     <row r="27" spans="2:14" ht="28.8" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="41" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -2525,8 +2646,8 @@
       <c r="B28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="39"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="41"/>
       <c r="E28" s="3" t="s">
         <v>78</v>
       </c>
@@ -2562,8 +2683,8 @@
       <c r="B29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="41"/>
       <c r="E29" s="3" t="s">
         <v>61</v>
       </c>
@@ -2599,8 +2720,8 @@
       <c r="B30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="39"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="3" t="s">
         <v>64</v>
       </c>
@@ -2636,8 +2757,8 @@
       <c r="B31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="39"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="3" t="s">
         <v>68</v>
       </c>
@@ -2657,13 +2778,13 @@
         <v>12</v>
       </c>
       <c r="K31" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>12</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N31" s="10" t="s">
         <v>12</v>
@@ -2673,8 +2794,8 @@
       <c r="B32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="39"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="41"/>
       <c r="E32" s="14" t="s">
         <v>71</v>
       </c>
@@ -2710,8 +2831,8 @@
       <c r="B33" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="39"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="41"/>
       <c r="E33" s="3" t="s">
         <v>74</v>
       </c>
@@ -2747,8 +2868,8 @@
       <c r="B34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="39"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="41"/>
       <c r="E34" s="3" t="s">
         <v>56</v>
       </c>
@@ -2774,7 +2895,7 @@
         <v>30</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N34" s="10" t="s">
         <v>12</v>
@@ -2784,8 +2905,8 @@
       <c r="B35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="39"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="41"/>
       <c r="E35" s="3" t="s">
         <v>80</v>
       </c>
@@ -2805,7 +2926,7 @@
         <v>12</v>
       </c>
       <c r="K35" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L35" s="13" t="s">
         <v>30</v>
@@ -2821,8 +2942,8 @@
       <c r="B36" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="39"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="41"/>
       <c r="E36" s="15" t="s">
         <v>82</v>
       </c>
@@ -2842,7 +2963,7 @@
         <v>12</v>
       </c>
       <c r="K36" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L36" s="13" t="s">
         <v>30</v>
@@ -2854,7 +2975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:14" s="40" customFormat="1"/>
+    <row r="37" spans="2:14" s="33" customFormat="1"/>
     <row r="38" spans="2:14" ht="43.2">
       <c r="B38" s="6" t="s">
         <v>83</v>
@@ -2896,7 +3017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:14" s="40" customFormat="1"/>
+    <row r="39" spans="2:14" s="33" customFormat="1"/>
     <row r="40" spans="2:14" ht="15" customHeight="1">
       <c r="B40" s="6" t="s">
         <v>88</v>
@@ -2938,15 +3059,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:14" s="40" customFormat="1"/>
+    <row r="41" spans="2:14" s="33" customFormat="1"/>
     <row r="42" spans="2:14" ht="14.4" customHeight="1">
       <c r="B42" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="41" t="s">
         <v>95</v>
       </c>
       <c r="E42" s="3">
@@ -2967,14 +3088,14 @@
       <c r="J42" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K42" s="37" t="s">
-        <v>146</v>
+      <c r="K42" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="L42" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M42" s="37" t="s">
-        <v>146</v>
+      <c r="M42" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="N42" s="19" t="s">
         <v>96</v>
@@ -2984,8 +3105,8 @@
       <c r="B43" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
       <c r="E43" s="3">
         <v>1</v>
       </c>
@@ -3004,11 +3125,11 @@
       <c r="J43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="37"/>
+      <c r="K43" s="36"/>
       <c r="L43" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M43" s="37"/>
+      <c r="M43" s="36"/>
       <c r="N43" s="19" t="s">
         <v>96</v>
       </c>
@@ -3017,8 +3138,8 @@
       <c r="B44" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
       <c r="E44" s="3">
         <v>1000</v>
       </c>
@@ -3037,11 +3158,11 @@
       <c r="J44" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K44" s="37"/>
+      <c r="K44" s="36"/>
       <c r="L44" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M44" s="37"/>
+      <c r="M44" s="36"/>
       <c r="N44" s="19" t="s">
         <v>96</v>
       </c>
@@ -3050,8 +3171,8 @@
       <c r="B45" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
       <c r="E45" s="3">
         <v>1234.3209999999999</v>
       </c>
@@ -3070,11 +3191,11 @@
       <c r="J45" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K45" s="37"/>
+      <c r="K45" s="36"/>
       <c r="L45" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M45" s="37"/>
+      <c r="M45" s="36"/>
       <c r="N45" s="19" t="s">
         <v>96</v>
       </c>
@@ -3083,8 +3204,8 @@
       <c r="B46" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
       <c r="E46" s="19" t="s">
         <v>101</v>
       </c>
@@ -3103,11 +3224,11 @@
       <c r="J46" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K46" s="37"/>
+      <c r="K46" s="36"/>
       <c r="L46" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M46" s="37"/>
+      <c r="M46" s="36"/>
       <c r="N46" s="19" t="s">
         <v>96</v>
       </c>
@@ -3125,10 +3246,10 @@
       <c r="B48" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="39" t="s">
+      <c r="D48" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E48" s="3">
@@ -3149,14 +3270,14 @@
       <c r="J48" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K48" s="37" t="s">
-        <v>146</v>
+      <c r="K48" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="L48" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M48" s="37" t="s">
-        <v>146</v>
+      <c r="M48" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="N48" s="19" t="s">
         <v>96</v>
@@ -3166,8 +3287,8 @@
       <c r="B49" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="39"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="41"/>
       <c r="E49" s="3">
         <v>0.5</v>
       </c>
@@ -3186,11 +3307,11 @@
       <c r="J49" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K49" s="38"/>
+      <c r="K49" s="37"/>
       <c r="L49" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M49" s="38"/>
+      <c r="M49" s="37"/>
       <c r="N49" s="19" t="s">
         <v>96</v>
       </c>
@@ -3199,8 +3320,8 @@
       <c r="B50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="39"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="41"/>
       <c r="E50" s="3">
         <v>1</v>
       </c>
@@ -3219,11 +3340,11 @@
       <c r="J50" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K50" s="38"/>
+      <c r="K50" s="37"/>
       <c r="L50" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M50" s="38"/>
+      <c r="M50" s="37"/>
       <c r="N50" s="19" t="s">
         <v>96</v>
       </c>
@@ -3232,8 +3353,8 @@
       <c r="B51" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="39"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="41"/>
       <c r="E51" s="3">
         <v>0.75</v>
       </c>
@@ -3252,11 +3373,11 @@
       <c r="J51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K51" s="38"/>
+      <c r="K51" s="37"/>
       <c r="L51" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M51" s="38"/>
+      <c r="M51" s="37"/>
       <c r="N51" s="19" t="s">
         <v>96</v>
       </c>
@@ -3265,8 +3386,8 @@
       <c r="B52" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="39"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="41"/>
       <c r="E52" s="19" t="s">
         <v>108</v>
       </c>
@@ -3285,24 +3406,24 @@
       <c r="J52" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K52" s="38"/>
+      <c r="K52" s="37"/>
       <c r="L52" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M52" s="38"/>
+      <c r="M52" s="37"/>
       <c r="N52" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="2:14" s="40" customFormat="1"/>
+    <row r="53" spans="2:14" s="33" customFormat="1"/>
     <row r="54" spans="2:14" ht="14.4" customHeight="1">
       <c r="B54" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="39" t="s">
+      <c r="C54" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D54" s="39" t="s">
+      <c r="D54" s="41" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="19" t="s">
@@ -3323,14 +3444,14 @@
       <c r="J54" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K54" s="35" t="s">
-        <v>138</v>
+      <c r="K54" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="L54" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M54" s="35" t="s">
-        <v>138</v>
+      <c r="M54" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="N54" s="19" t="s">
         <v>96</v>
@@ -3340,8 +3461,8 @@
       <c r="B55" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
       <c r="E55" s="19" t="s">
         <v>113</v>
       </c>
@@ -3360,11 +3481,11 @@
       <c r="J55" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="35"/>
+      <c r="K55" s="34"/>
       <c r="L55" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M55" s="35"/>
+      <c r="M55" s="34"/>
       <c r="N55" s="19" t="s">
         <v>96</v>
       </c>
@@ -3373,8 +3494,8 @@
       <c r="B56" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
       <c r="E56" s="19" t="s">
         <v>115</v>
       </c>
@@ -3393,11 +3514,11 @@
       <c r="J56" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K56" s="35"/>
+      <c r="K56" s="34"/>
       <c r="L56" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M56" s="35"/>
+      <c r="M56" s="34"/>
       <c r="N56" s="19" t="s">
         <v>96</v>
       </c>
@@ -3406,8 +3527,8 @@
       <c r="B57" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
       <c r="E57" s="19" t="s">
         <v>117</v>
       </c>
@@ -3426,11 +3547,11 @@
       <c r="J57" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="K57" s="35"/>
+      <c r="K57" s="34"/>
       <c r="L57" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M57" s="35"/>
+      <c r="M57" s="34"/>
       <c r="N57" s="19" t="s">
         <v>96</v>
       </c>
@@ -3439,8 +3560,8 @@
       <c r="B58" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
       <c r="E58" s="19" t="s">
         <v>120</v>
       </c>
@@ -3459,11 +3580,11 @@
       <c r="J58" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K58" s="35"/>
+      <c r="K58" s="34"/>
       <c r="L58" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M58" s="35"/>
+      <c r="M58" s="34"/>
       <c r="N58" s="19" t="s">
         <v>96</v>
       </c>
@@ -3472,8 +3593,8 @@
       <c r="B59" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
       <c r="E59" s="19" t="s">
         <v>122</v>
       </c>
@@ -3492,11 +3613,11 @@
       <c r="J59" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K59" s="35"/>
+      <c r="K59" s="34"/>
       <c r="L59" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M59" s="35"/>
+      <c r="M59" s="34"/>
       <c r="N59" s="19" t="s">
         <v>96</v>
       </c>
@@ -3504,11 +3625,11 @@
     <row r="60" spans="2:14" s="26" customFormat="1"/>
     <row r="61" spans="2:14" s="25" customFormat="1" ht="14.4" customHeight="1">
       <c r="B61" s="11"/>
-      <c r="C61" s="33" t="s">
+      <c r="C61" s="42" t="s">
         <v>123</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E61" s="23" t="s">
         <v>125</v>
@@ -3529,13 +3650,13 @@
         <v>96</v>
       </c>
       <c r="K61" s="25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>12</v>
       </c>
       <c r="M61" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N61" s="10" t="s">
         <v>12</v>
@@ -3543,8 +3664,8 @@
     </row>
     <row r="62" spans="2:14" s="25" customFormat="1">
       <c r="B62" s="11"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
       <c r="E62" s="23" t="s">
         <v>126</v>
       </c>
@@ -3564,13 +3685,13 @@
         <v>96</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>12</v>
       </c>
       <c r="M62" s="25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="N62" s="10" t="s">
         <v>12</v>
@@ -3578,8 +3699,8 @@
     </row>
     <row r="63" spans="2:14" s="25" customFormat="1">
       <c r="B63" s="11"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
       <c r="E63" s="23" t="s">
         <v>127</v>
       </c>
@@ -3599,13 +3720,13 @@
         <v>96</v>
       </c>
       <c r="K63" s="25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>12</v>
       </c>
       <c r="M63" s="25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N63" s="10" t="s">
         <v>12</v>
@@ -3613,8 +3734,8 @@
     </row>
     <row r="64" spans="2:14" s="25" customFormat="1" ht="43.2">
       <c r="B64" s="11"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
       <c r="E64" s="23" t="s">
         <v>128</v>
       </c>
@@ -3634,13 +3755,13 @@
         <v>96</v>
       </c>
       <c r="K64" s="25" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L64" s="13" t="s">
         <v>30</v>
       </c>
       <c r="M64" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N64" s="10" t="s">
         <v>12</v>
@@ -3648,8 +3769,8 @@
     </row>
     <row r="65" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B65" s="11"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="42"/>
       <c r="E65" s="23" t="s">
         <v>129</v>
       </c>
@@ -3669,13 +3790,13 @@
         <v>96</v>
       </c>
       <c r="K65" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L65" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M65" s="25" t="s">
-        <v>152</v>
+      <c r="M65" s="46" t="s">
+        <v>161</v>
       </c>
       <c r="N65" s="13" t="s">
         <v>30</v>
@@ -3683,8 +3804,8 @@
     </row>
     <row r="66" spans="2:14" s="25" customFormat="1" ht="28.05" customHeight="1">
       <c r="B66" s="11"/>
-      <c r="C66" s="33"/>
-      <c r="D66" s="33"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
       <c r="E66" s="23" t="s">
         <v>130</v>
       </c>
@@ -3704,27 +3825,27 @@
         <v>96</v>
       </c>
       <c r="K66" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L66" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M66" s="25" t="s">
-        <v>152</v>
+      <c r="M66" s="46" t="s">
+        <v>161</v>
       </c>
       <c r="N66" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="2:14" s="25" customFormat="1" ht="43.2">
+    <row r="67" spans="2:14" s="25" customFormat="1" ht="28.8">
       <c r="B67" s="11"/>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
       <c r="E67" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="F67" s="23" t="s">
-        <v>135</v>
+      <c r="F67" s="45" t="s">
+        <v>159</v>
       </c>
       <c r="G67" s="19" t="s">
         <v>96</v>
@@ -3739,13 +3860,13 @@
         <v>96</v>
       </c>
       <c r="K67" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L67" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M67" s="25" t="s">
-        <v>152</v>
+      <c r="M67" s="46" t="s">
+        <v>162</v>
       </c>
       <c r="N67" s="13" t="s">
         <v>30</v>
@@ -3753,8 +3874,8 @@
     </row>
     <row r="68" spans="2:14" s="25" customFormat="1">
       <c r="B68" s="11"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="33"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
       <c r="E68" s="23" t="s">
         <v>51</v>
       </c>
@@ -3774,24 +3895,24 @@
         <v>96</v>
       </c>
       <c r="K68" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="L68" s="10" t="s">
         <v>12</v>
       </c>
       <c r="M68" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="N68" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="2:14" s="34" customFormat="1"/>
+    <row r="69" spans="2:14" s="43" customFormat="1"/>
     <row r="70" spans="2:14" ht="14.4" customHeight="1">
-      <c r="C70" s="33" t="s">
+      <c r="C70" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="D70" s="33" t="s">
+      <c r="D70" s="42" t="s">
         <v>132</v>
       </c>
       <c r="E70" s="23" t="s">
@@ -3813,21 +3934,21 @@
         <v>96</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>12</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N70" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="71" spans="2:14">
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="42"/>
       <c r="E71" s="23" t="s">
         <v>126</v>
       </c>
@@ -3860,8 +3981,8 @@
       </c>
     </row>
     <row r="72" spans="2:14">
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
+      <c r="C72" s="42"/>
+      <c r="D72" s="42"/>
       <c r="E72" s="23" t="s">
         <v>127</v>
       </c>
@@ -3894,8 +4015,8 @@
       </c>
     </row>
     <row r="73" spans="2:14" ht="57.6">
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
       <c r="E73" s="23" t="s">
         <v>128</v>
       </c>
@@ -3915,7 +4036,7 @@
         <v>96</v>
       </c>
       <c r="K73" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L73" s="13" t="s">
         <v>30</v>
@@ -3928,8 +4049,8 @@
       </c>
     </row>
     <row r="74" spans="2:14" ht="28.8">
-      <c r="C74" s="33"/>
-      <c r="D74" s="33"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="42"/>
       <c r="E74" s="23" t="s">
         <v>129</v>
       </c>
@@ -3949,21 +4070,21 @@
         <v>96</v>
       </c>
       <c r="K74" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L74" s="13" t="s">
         <v>30</v>
       </c>
       <c r="M74" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N74" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="75" spans="2:14" ht="28.8">
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
       <c r="E75" s="23" t="s">
         <v>130</v>
       </c>
@@ -3983,26 +4104,26 @@
         <v>96</v>
       </c>
       <c r="K75" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L75" s="13" t="s">
         <v>30</v>
       </c>
       <c r="M75" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N75" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="76" spans="2:14" ht="43.2">
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
       <c r="E76" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="F76" s="23" t="s">
-        <v>135</v>
+      <c r="F76" s="45" t="s">
+        <v>160</v>
       </c>
       <c r="G76" s="19" t="s">
         <v>96</v>
@@ -4017,21 +4138,21 @@
         <v>96</v>
       </c>
       <c r="K76" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L76" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="M76" s="31" t="s">
-        <v>148</v>
+      <c r="M76" s="45" t="s">
+        <v>163</v>
       </c>
       <c r="N76" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="77" spans="2:14">
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
       <c r="E77" s="23" t="s">
         <v>51</v>
       </c>
@@ -4073,6 +4194,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C70:C77"/>
+    <mergeCell ref="D70:D77"/>
+    <mergeCell ref="A69:XFD69"/>
+    <mergeCell ref="M54:M59"/>
+    <mergeCell ref="K16:K25"/>
+    <mergeCell ref="K54:K59"/>
+    <mergeCell ref="K42:K46"/>
+    <mergeCell ref="K48:K52"/>
+    <mergeCell ref="C16:C25"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="C61:C68"/>
+    <mergeCell ref="D61:D68"/>
+    <mergeCell ref="C48:C52"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="D16:D25"/>
+    <mergeCell ref="D27:D36"/>
+    <mergeCell ref="D42:D46"/>
+    <mergeCell ref="D48:D52"/>
+    <mergeCell ref="A26:XFD26"/>
+    <mergeCell ref="A37:XFD37"/>
+    <mergeCell ref="A39:XFD39"/>
+    <mergeCell ref="A41:XFD41"/>
     <mergeCell ref="A53:XFD53"/>
     <mergeCell ref="M16:M25"/>
     <mergeCell ref="M42:M46"/>
@@ -4089,32 +4236,6 @@
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="K4:K7"/>
     <mergeCell ref="K9:K14"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="A26:XFD26"/>
-    <mergeCell ref="A37:XFD37"/>
-    <mergeCell ref="A39:XFD39"/>
-    <mergeCell ref="A41:XFD41"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="D16:D25"/>
-    <mergeCell ref="D27:D36"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="C70:C77"/>
-    <mergeCell ref="D70:D77"/>
-    <mergeCell ref="A69:XFD69"/>
-    <mergeCell ref="M54:M59"/>
-    <mergeCell ref="K16:K25"/>
-    <mergeCell ref="K54:K59"/>
-    <mergeCell ref="K42:K46"/>
-    <mergeCell ref="K48:K52"/>
-    <mergeCell ref="C16:C25"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="C61:C68"/>
-    <mergeCell ref="D61:D68"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="C54:C59"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>